<commit_message>
Fix - Fixed birthday input in the spreadshee.
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VRG_9\Escritorio\Python\ProyectoBolivia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECDD005-B421-46B3-A903-F8189C798C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D242225E-E80E-4541-A993-EAF5413974A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74D8D854-A4EC-4F8A-8E32-A965954A1EC9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Nombre</t>
   </si>
@@ -86,9 +86,6 @@
     <t>YNGARTH KATIUSKA</t>
   </si>
   <si>
-    <t>14/9/1977</t>
-  </si>
-  <si>
     <t>JOSE1994WIN@GMAIL.COM</t>
   </si>
   <si>
@@ -204,6 +201,18 @@
   </si>
   <si>
     <t>Origen_Fondos</t>
+  </si>
+  <si>
+    <t>01/09/2017</t>
+  </si>
+  <si>
+    <t>20/02/1990</t>
+  </si>
+  <si>
+    <t>24/12/1999</t>
+  </si>
+  <si>
+    <t>14/09/1977</t>
   </si>
 </sst>
 </file>
@@ -268,10 +277,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -591,16 +600,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901B2EB3-F866-4EDE-9274-D55BD9B51CBB}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H23" sqref="H22:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.44140625" bestFit="1" customWidth="1"/>
@@ -613,37 +623,37 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>
@@ -662,8 +672,8 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5">
-        <v>37750</v>
+      <c r="D2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E2">
         <v>14749250</v>
@@ -704,7 +714,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="E3">
         <v>4707287</v>
@@ -716,13 +726,13 @@
         <v>76692876</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -736,16 +746,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5">
-        <v>34892</v>
+      <c r="D4" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="E4">
         <v>7831456</v>
@@ -757,10 +767,10 @@
         <v>75501277</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -777,16 +787,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="E5">
         <v>3905430</v>
@@ -798,19 +808,19 @@
         <v>74188233</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
         <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" t="s">
-        <v>29</v>
       </c>
       <c r="M5">
         <v>1000</v>
@@ -818,16 +828,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="E6">
         <v>15987987</v>
@@ -839,7 +849,7 @@
         <v>64452817</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -851,7 +861,7 @@
         <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6">
         <v>1000</v>
@@ -859,31 +869,31 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="E7">
         <v>11375638</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7">
         <v>76633552</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -900,37 +910,40 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="5">
-        <v>34525</v>
+      <c r="D8" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="E8">
         <v>13132749</v>
       </c>
       <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8">
+        <v>76633552</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="I8" t="s">
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" t="s">
         <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M8">
         <v>1000</v>
@@ -940,11 +953,22 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D10" s="5"/>
       <c r="H10" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F13" s="6"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F16" s="6"/>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>